<commit_message>
Changed a subject's info
</commit_message>
<xml_diff>
--- a/NFB analysis subjects 7.1.19.xlsx
+++ b/NFB analysis subjects 7.1.19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac637-jbj-100/Desktop/Neurofeedback/BIDS_TEST/matlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFE5A2B-74F1-6241-9AA8-A4D46AD27814}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0A691E-FEA4-4A4A-811C-7B32781C0236}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9500" yWindow="1100" windowWidth="27760" windowHeight="18140" xr2:uid="{2B411EA9-DD6E-D549-B621-B50633F7B67E}"/>
+    <workbookView xWindow="22860" yWindow="2240" windowWidth="27760" windowHeight="18140" xr2:uid="{2B411EA9-DD6E-D549-B621-B50633F7B67E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -781,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E017A16F-C8E0-C540-A08B-6028006FC870}">
   <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2921,7 +2921,7 @@
         <v>63</v>
       </c>
       <c r="B77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77" s="1">
         <v>1</v>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="H77" s="2" t="str">
         <f>IF(AND(B77=1,C77=1,D77=1,E77=0,F77=0), "YES","NO")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>